<commit_message>
Added JWT, NgxBootstrap And Theme
</commit_message>
<xml_diff>
--- a/AngularWithC#.xlsx
+++ b/AngularWithC#.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7515"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
   <si>
     <t>Tools for developing</t>
   </si>
@@ -206,13 +206,37 @@
   </si>
   <si>
     <t>Install angular CLI</t>
+  </si>
+  <si>
+    <t>https://www.npmjs.com/package/ngx-toastr</t>
+  </si>
+  <si>
+    <t>ngx-toastr</t>
+  </si>
+  <si>
+    <t>auth0/angular-jwt</t>
+  </si>
+  <si>
+    <t>This library provides an HttpInterceptor which automatically attaches a JSON Web Token to HttpClient requests.</t>
+  </si>
+  <si>
+    <t>https://www.npmjs.com/package/@auth0/angular-jwt</t>
+  </si>
+  <si>
+    <t>https://bootswatch.com/</t>
+  </si>
+  <si>
+    <t>Free themes for Bootstrap</t>
+  </si>
+  <si>
+    <t>Bootswatch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,6 +259,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -275,20 +307,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -347,7 +382,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -382,7 +417,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -591,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,268 +659,303 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
       <c r="B4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" t="s">
-        <v>49</v>
+        <v>70</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>52</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-    </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
-        <v>4</v>
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>6</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C13" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>20</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C14" t="s">
         <v>23</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D14" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>32</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D20" t="s">
-        <v>25</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C24" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="2" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C25" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="2"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B27" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>8</v>
-      </c>
-      <c r="C28" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>13</v>
+        <v>57</v>
+      </c>
+      <c r="C29" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>33</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>62</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B37" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>61</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B38" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>44</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B43" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>56</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B44" t="s">
         <v>55</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C9" r:id="rId1"/>
+    <hyperlink ref="C4" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added Thumbnail Gallery To Modal
</commit_message>
<xml_diff>
--- a/AngularWithC#.xlsx
+++ b/AngularWithC#.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="77">
   <si>
     <t>Tools for developing</t>
   </si>
@@ -239,6 +239,15 @@
   </si>
   <si>
     <t>https://www.json-generator.com/</t>
+  </si>
+  <si>
+    <t>hyphen</t>
+  </si>
+  <si>
+    <t>https://www.npmjs.com/package/hyphen</t>
+  </si>
+  <si>
+    <t>This is a text hyphenation library, based on Franklin M. Liang's hyphenation algorithm. In core of the algorithm lies a set of hyphenation patterns. They are extracted from hand-hyphenated dictionaries. Patterns for this library were taken from ctan.org and ported to Javascript.</t>
   </si>
 </sst>
 </file>
@@ -635,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,238 +745,249 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="B12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
+    <row r="20" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D24" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" t="s">
-        <v>38</v>
+        <v>59</v>
+      </c>
+      <c r="D25" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C26" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="2"/>
+      <c r="B27" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30" t="s">
-        <v>58</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>14</v>
+        <v>57</v>
+      </c>
+      <c r="C31" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>8</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+    <row r="34" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>33</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>62</v>
-      </c>
-      <c r="B38" t="s">
-        <v>16</v>
-      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>62</v>
+      </c>
+      <c r="B39" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>61</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>44</v>
-      </c>
-      <c r="B44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>56</v>
+      </c>
+      <c r="B46" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>71</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>72</v>
       </c>
     </row>
@@ -976,9 +996,10 @@
     <hyperlink ref="C10" r:id="rId1"/>
     <hyperlink ref="C5" r:id="rId2"/>
     <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="C12" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added Sortable On FrontEnd
</commit_message>
<xml_diff>
--- a/AngularWithC#.xlsx
+++ b/AngularWithC#.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="86">
   <si>
     <t>Tools for developing</t>
   </si>
@@ -263,6 +263,18 @@
   </si>
   <si>
     <t>Angular 9|8|7 | Show Global Spinner/ Loader on HTTP calls in few steps using Angular Interceptors in Angular 4.3+</t>
+  </si>
+  <si>
+    <t>dotnet ef database update AddEventLanguages</t>
+  </si>
+  <si>
+    <t>Swich To Migration</t>
+  </si>
+  <si>
+    <t>dotnet ef migrations remove</t>
+  </si>
+  <si>
+    <t>Remove last migration</t>
   </si>
 </sst>
 </file>
@@ -662,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -942,93 +954,109 @@
         <v>36</v>
       </c>
     </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>82</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="B38" t="s">
+        <v>84</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>62</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B41" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>61</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B42" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>44</v>
-      </c>
-      <c r="B45" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>56</v>
-      </c>
-      <c r="B46" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>44</v>
+      </c>
+      <c r="B47" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>56</v>
+      </c>
+      <c r="B48" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>71</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B49" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-    </row>
-    <row r="50" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+    </row>
+    <row r="52" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B52" s="5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>81</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B53" s="4" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1038,8 +1066,8 @@
     <hyperlink ref="C5" r:id="rId2"/>
     <hyperlink ref="B3" r:id="rId3"/>
     <hyperlink ref="C12" r:id="rId4"/>
-    <hyperlink ref="B50" r:id="rId5"/>
-    <hyperlink ref="B51" r:id="rId6"/>
+    <hyperlink ref="B52" r:id="rId5"/>
+    <hyperlink ref="B53" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId7"/>

</xml_diff>

<commit_message>
Fix Search By Name
</commit_message>
<xml_diff>
--- a/AngularWithC#.xlsx
+++ b/AngularWithC#.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7515"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="86">
   <si>
     <t>Tools for developing</t>
   </si>
@@ -269,12 +269,32 @@
   </si>
   <si>
     <t>Run External</t>
+  </si>
+  <si>
+    <t>Reversing A Migration.</t>
+  </si>
+  <si>
+    <r>
+      <t>dotnet ef database update CreateMigration</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -351,7 +371,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -361,6 +381,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -424,7 +450,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -459,7 +485,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -668,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -948,101 +974,109 @@
         <v>36</v>
       </c>
     </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="B38" t="s">
+        <v>72</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>82</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>62</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B42" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>61</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B43" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>44</v>
-      </c>
-      <c r="B45" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>56</v>
-      </c>
-      <c r="B46" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>71</v>
-      </c>
-      <c r="B47" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>83</v>
+        <v>44</v>
       </c>
       <c r="B48" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>56</v>
+      </c>
+      <c r="B49" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-    </row>
-    <row r="51" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+    </row>
+    <row r="55" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B55" s="5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>81</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B56" s="4" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1052,8 +1086,8 @@
     <hyperlink ref="C5" r:id="rId2"/>
     <hyperlink ref="B3" r:id="rId3"/>
     <hyperlink ref="C12" r:id="rId4"/>
-    <hyperlink ref="B51" r:id="rId5"/>
-    <hyperlink ref="B52" r:id="rId6"/>
+    <hyperlink ref="B55" r:id="rId5"/>
+    <hyperlink ref="B56" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId7"/>

</xml_diff>